<commit_message>
Final changes to analysis files
Co-Authored-By: Melissa Pérez <84192851+MelissaPerez09@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/analysis/DP.xlsx
+++ b/analysis/DP.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\Proyecto02-CC3041\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\1-UVG-2024\Algoritmos\proyecto2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60B6D6A-F0D1-4999-B75E-A75A231BAB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79B6328-1129-417A-A45A-3958705BA2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1116,6 +1119,1116 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Complejidad (O(n⋅m)) vs Nodos</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-GT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>O(n⋅m)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.14832294226570053"/>
+                  <c:y val="0.1156435394459253"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-GT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[1]Sheet1!$A$2:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[1]Sheet1!$D$2:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>459</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>477</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>477</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>441</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>441</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>102</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-110A-451E-A6FB-AC0E0F48E537}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1200838255"/>
+        <c:axId val="1200836815"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1200838255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1200836815"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1200836815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1200838255"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-GT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Complejidad (O(n⋅m)) vs</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Aristas</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-GT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>O(n⋅m)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.7062176952813833E-2"/>
+                  <c:y val="0.14888787551548871"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-GT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[1]Sheet1!$B$2:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[1]Sheet1!$D$2:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>459</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>477</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>477</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>441</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>441</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>102</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B8B8-4377-AEFE-0188C21162B6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1200838255"/>
+        <c:axId val="1200836815"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1200838255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1200836815"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1200836815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1200838255"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-GT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
   <a:schemeClr val="accent3"/>
@@ -1128,6 +2241,18 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+  <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+  <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
   <cs:axisTitle>
@@ -1649,6 +2774,1046 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2242,7 +4407,435 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>496455</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>34636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>184141</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>165238</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4836709-5D03-41D5-8EAA-D32DA07BCB64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>46182</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>92363</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>345777</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>38236</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98777789-9028-4182-9536-F548A70E4F8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="D1" t="str">
+            <v>O(n⋅m)</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>7</v>
+          </cell>
+          <cell r="B2">
+            <v>26</v>
+          </cell>
+          <cell r="D2">
+            <v>182</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>9</v>
+          </cell>
+          <cell r="B3">
+            <v>52</v>
+          </cell>
+          <cell r="D3">
+            <v>468</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>5</v>
+          </cell>
+          <cell r="B4">
+            <v>12</v>
+          </cell>
+          <cell r="D4">
+            <v>60</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>9</v>
+          </cell>
+          <cell r="B5">
+            <v>54</v>
+          </cell>
+          <cell r="D5">
+            <v>486</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>7</v>
+          </cell>
+          <cell r="B6">
+            <v>28</v>
+          </cell>
+          <cell r="D6">
+            <v>196</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>9</v>
+          </cell>
+          <cell r="B7">
+            <v>52</v>
+          </cell>
+          <cell r="D7">
+            <v>468</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>8</v>
+          </cell>
+          <cell r="B8">
+            <v>39</v>
+          </cell>
+          <cell r="D8">
+            <v>312</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>6</v>
+          </cell>
+          <cell r="B9">
+            <v>17</v>
+          </cell>
+          <cell r="D9">
+            <v>102</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>6</v>
+          </cell>
+          <cell r="B10">
+            <v>20</v>
+          </cell>
+          <cell r="D10">
+            <v>120</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>9</v>
+          </cell>
+          <cell r="B11">
+            <v>48</v>
+          </cell>
+          <cell r="D11">
+            <v>432</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>5</v>
+          </cell>
+          <cell r="B12">
+            <v>13</v>
+          </cell>
+          <cell r="D12">
+            <v>65</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>9</v>
+          </cell>
+          <cell r="B13">
+            <v>51</v>
+          </cell>
+          <cell r="D13">
+            <v>459</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>7</v>
+          </cell>
+          <cell r="B14">
+            <v>30</v>
+          </cell>
+          <cell r="D14">
+            <v>210</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>7</v>
+          </cell>
+          <cell r="B15">
+            <v>28</v>
+          </cell>
+          <cell r="D15">
+            <v>196</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>9</v>
+          </cell>
+          <cell r="B16">
+            <v>53</v>
+          </cell>
+          <cell r="D16">
+            <v>477</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>7</v>
+          </cell>
+          <cell r="B17">
+            <v>27</v>
+          </cell>
+          <cell r="D17">
+            <v>189</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>9</v>
+          </cell>
+          <cell r="B18">
+            <v>53</v>
+          </cell>
+          <cell r="D18">
+            <v>477</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>6</v>
+          </cell>
+          <cell r="B19">
+            <v>18</v>
+          </cell>
+          <cell r="D19">
+            <v>108</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>7</v>
+          </cell>
+          <cell r="B20">
+            <v>27</v>
+          </cell>
+          <cell r="D20">
+            <v>189</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>6</v>
+          </cell>
+          <cell r="B21">
+            <v>16</v>
+          </cell>
+          <cell r="D21">
+            <v>96</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>7</v>
+          </cell>
+          <cell r="B22">
+            <v>25</v>
+          </cell>
+          <cell r="D22">
+            <v>175</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>5</v>
+          </cell>
+          <cell r="B23">
+            <v>14</v>
+          </cell>
+          <cell r="D23">
+            <v>70</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>7</v>
+          </cell>
+          <cell r="B24">
+            <v>25</v>
+          </cell>
+          <cell r="D24">
+            <v>175</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>10</v>
+          </cell>
+          <cell r="B25">
+            <v>53</v>
+          </cell>
+          <cell r="D25">
+            <v>530</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>5</v>
+          </cell>
+          <cell r="B26">
+            <v>13</v>
+          </cell>
+          <cell r="D26">
+            <v>65</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>9</v>
+          </cell>
+          <cell r="B27">
+            <v>49</v>
+          </cell>
+          <cell r="D27">
+            <v>441</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>7</v>
+          </cell>
+          <cell r="B28">
+            <v>26</v>
+          </cell>
+          <cell r="D28">
+            <v>182</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>9</v>
+          </cell>
+          <cell r="B29">
+            <v>50</v>
+          </cell>
+          <cell r="D29">
+            <v>450</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>9</v>
+          </cell>
+          <cell r="B30">
+            <v>49</v>
+          </cell>
+          <cell r="D30">
+            <v>441</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>6</v>
+          </cell>
+          <cell r="B31">
+            <v>17</v>
+          </cell>
+          <cell r="D31">
+            <v>102</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2533,7 +5126,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+      <selection activeCell="Z12" sqref="Z12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>